<commit_message>
The changes have made do not have a significant impact
</commit_message>
<xml_diff>
--- a/VytrackTestUsers.xlsx
+++ b/VytrackTestUsers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\myuser\IdeaProjects\CybertekTestNGProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D79DB753-77C1-483B-A8E4-5B1AC852B74D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB61FD1A-D36C-4877-A204-DF5AC6B135E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{506372D9-39D2-EA47-AA3D-ABD5428ED2AB}"/>
   </bookViews>
@@ -22,7 +22,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3912" uniqueCount="1479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3897" uniqueCount="1479">
   <si>
     <t>username</t>
   </si>
@@ -4479,7 +4479,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -4827,17 +4826,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D70E95-9193-2444-8F5D-57688B5675B2}">
   <dimension ref="A1:E302"/>
   <sheetViews>
-    <sheetView topLeftCell="A212" zoomScale="200" workbookViewId="0">
+    <sheetView topLeftCell="B40" zoomScale="200" workbookViewId="0">
       <selection activeCell="A231" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="1" max="1" width="15.69921875" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4854,7 +4853,7 @@
         <v>1478</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -4868,7 +4867,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -4882,7 +4881,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -4896,7 +4895,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -4910,7 +4909,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4924,7 +4923,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4938,7 +4937,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -4952,7 +4951,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -4966,7 +4965,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -4980,7 +4979,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -4994,7 +4993,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -5008,7 +5007,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -5022,7 +5021,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -5036,7 +5035,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -5050,7 +5049,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -9080,8 +9079,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -9419,8 +9418,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -13666,8 +13665,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -14005,8 +14004,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -18246,14 +18245,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C30F00C-C683-0548-B7C4-02FB1EBCAEF1}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="200" workbookViewId="0">
+      <selection activeCell="F16" sqref="F2:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.69921875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.796875" collapsed="true"/>
+    <col min="2" max="2" width="15.69921875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.796875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -18292,9 +18291,6 @@
       <c r="E2" t="s">
         <v>305</v>
       </c>
-      <c r="F2" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -18312,9 +18308,6 @@
       <c r="E3" t="s">
         <v>725</v>
       </c>
-      <c r="F3" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -18332,9 +18325,6 @@
       <c r="E4" t="s">
         <v>307</v>
       </c>
-      <c r="F4" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
@@ -18352,9 +18342,6 @@
       <c r="E5" t="s">
         <v>610</v>
       </c>
-      <c r="F5" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
@@ -18372,9 +18359,6 @@
       <c r="E6" t="s">
         <v>1021</v>
       </c>
-      <c r="F6" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -18392,9 +18376,6 @@
       <c r="E7" t="s">
         <v>1274</v>
       </c>
-      <c r="F7" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -18412,9 +18393,6 @@
       <c r="E8" t="s">
         <v>337</v>
       </c>
-      <c r="F8" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -18432,9 +18410,6 @@
       <c r="E9" t="s">
         <v>796</v>
       </c>
-      <c r="F9" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
@@ -18452,9 +18427,6 @@
       <c r="E10" t="s">
         <v>644</v>
       </c>
-      <c r="F10" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -18472,9 +18444,6 @@
       <c r="E11" t="s">
         <v>586</v>
       </c>
-      <c r="F11" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -18492,9 +18461,6 @@
       <c r="E12" t="s">
         <v>1375</v>
       </c>
-      <c r="F12" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -18512,9 +18478,6 @@
       <c r="E13" t="s">
         <v>1001</v>
       </c>
-      <c r="F13" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
@@ -18532,9 +18495,6 @@
       <c r="E14" t="s">
         <v>1378</v>
       </c>
-      <c r="F14" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -18552,9 +18512,6 @@
       <c r="E15" t="s">
         <v>1379</v>
       </c>
-      <c r="F15" t="s">
-        <v>1477</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
@@ -18571,9 +18528,6 @@
       </c>
       <c r="E16" t="s">
         <v>1381</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>